<commit_message>
added stuff to code
</commit_message>
<xml_diff>
--- a/Analysis Codes/Experimental Data.xlsx
+++ b/Analysis Codes/Experimental Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\J lab\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\ME201617\ME Spring 2017\Final project\Analysis Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>RPM</t>
   </si>
@@ -66,16 +66,22 @@
     <t>Force (N)</t>
   </si>
   <si>
-    <t>P1 (inHg)</t>
+    <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">P2 (inHg) </t>
+    <t>Air density data obtained from WeatherForYou.com on April 30, 2017</t>
   </si>
   <si>
-    <t>P2 (inHg)</t>
+    <t>rho=</t>
   </si>
   <si>
-    <t>-</t>
+    <t>P1 (inH2O)</t>
+  </si>
+  <si>
+    <t>P2 (inH2O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2 (inH2O) </t>
   </si>
 </sst>
 </file>
@@ -174,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -193,15 +199,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -369,32 +366,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -403,10 +400,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,82 +412,79 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -499,10 +493,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,27 +505,30 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,31 +538,28 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -853,19 +847,21 @@
   </sheetPr>
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="16.42578125" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" customWidth="1"/>
@@ -876,54 +872,54 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-      <c r="J2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+      <c r="J2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="B3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="20"/>
       <c r="J3" s="3">
         <v>1.5</v>
       </c>
@@ -935,8 +931,8 @@
         <v>7.6200000000000009E-3</v>
       </c>
       <c r="M3" s="5">
-        <f>((2*9.81*1000*L3)/1.225)^0.5</f>
-        <v>11.047371097381735</v>
+        <f>((2*9.81*1000*L3)/1.2093)^0.5</f>
+        <v>11.118852288315432</v>
       </c>
       <c r="N3" s="4">
         <v>0.67</v>
@@ -946,27 +942,27 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>1.65</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <v>1.3</v>
       </c>
-      <c r="D4" s="23">
-        <f>L3</f>
-        <v>7.6200000000000009E-3</v>
-      </c>
-      <c r="E4" s="23">
-        <f>M3</f>
-        <v>11.047371097381735</v>
-      </c>
-      <c r="F4" s="23">
+      <c r="D4" s="22">
+        <f>(B4-C4)*0.0254</f>
+        <v>8.8899999999999969E-3</v>
+      </c>
+      <c r="E4" s="22">
+        <f>((2*9.81*1000*D4)/1.2093)^0.5</f>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F4" s="22">
         <v>3100</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="22">
         <v>0.5</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="3">
@@ -980,38 +976,38 @@
         <v>1.6509999999999997E-2</v>
       </c>
       <c r="M4" s="5">
-        <f t="shared" ref="M4:M8" si="1">((2*9.81*1000*L4)/1.225)^0.5</f>
-        <v>16.261289955609552</v>
+        <f t="shared" ref="M4:M8" si="1">((2*9.81*1000*L4)/1.2093)^0.5</f>
+        <v>16.366507419737342</v>
       </c>
       <c r="N4" s="4">
         <v>0.61</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>2</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <v>1.35</v>
       </c>
-      <c r="D5" s="23">
-        <f>(B5-C5)*0.0254</f>
+      <c r="D5" s="22">
+        <f t="shared" ref="D5:D15" si="2">(B5-C5)*0.0254</f>
         <v>1.6509999999999997E-2</v>
       </c>
-      <c r="E5" s="23">
-        <f>((2*9.81*1000*D5)/1.225)^0.5</f>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F5" s="23">
+      <c r="E5" s="22">
+        <f t="shared" ref="E5:E15" si="3">((2*9.81*1000*D5)/1.2093)^0.5</f>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F5" s="22">
         <v>3024</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="22">
         <v>1.25</v>
       </c>
-      <c r="H5" s="24"/>
+      <c r="H5" s="23"/>
       <c r="J5" s="3">
         <v>2.5</v>
       </c>
@@ -1024,37 +1020,37 @@
       </c>
       <c r="M5" s="5">
         <f t="shared" si="1"/>
-        <v>20.169647837221923</v>
+        <v>20.300154039594325</v>
       </c>
       <c r="N5" s="4">
         <v>0.5</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <v>1.5</v>
       </c>
-      <c r="D6" s="23">
-        <f>(B6-C6)*0.0254</f>
+      <c r="D6" s="22">
+        <f t="shared" si="2"/>
         <v>2.4130000000000002E-2</v>
       </c>
-      <c r="E6" s="23">
-        <f>((2*9.81*1000*D6)/1.225)^0.5</f>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F6" s="23">
+      <c r="E6" s="22">
+        <f t="shared" si="3"/>
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F6" s="22">
         <v>2950</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="22">
         <v>1.35</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="23"/>
       <c r="J6" s="3">
         <v>3</v>
       </c>
@@ -1067,37 +1063,37 @@
       </c>
       <c r="M6" s="5">
         <f t="shared" si="1"/>
-        <v>23.435013051728689</v>
+        <v>23.586647556238209</v>
       </c>
       <c r="N6" s="4">
         <v>0.4</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="22">
+      <c r="B7" s="21">
         <v>3</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="22">
         <v>1.6</v>
       </c>
-      <c r="D7" s="23">
-        <f>(B7-C7)*0.0254</f>
+      <c r="D7" s="22">
+        <f t="shared" si="2"/>
         <v>3.5559999999999994E-2</v>
       </c>
-      <c r="E7" s="23">
-        <f>((2*9.81*1000*D7)/1.225)^0.5</f>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F7" s="23">
+      <c r="E7" s="22">
+        <f t="shared" si="3"/>
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F7" s="22">
         <v>2800</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="22">
         <v>1.43</v>
       </c>
-      <c r="H7" s="24"/>
+      <c r="H7" s="23"/>
       <c r="J7" s="3">
         <v>3.5</v>
       </c>
@@ -1110,37 +1106,37 @@
       </c>
       <c r="M7" s="5">
         <f t="shared" si="1"/>
-        <v>26.298003338501509</v>
+        <v>26.468162608181515</v>
       </c>
       <c r="N7" s="4">
         <v>0.36</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>1.65</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <v>1.3</v>
       </c>
-      <c r="D8" s="26">
-        <f>(B8-C8)*0.0254</f>
+      <c r="D8" s="25">
+        <f t="shared" si="2"/>
         <v>8.8899999999999969E-3</v>
       </c>
-      <c r="E8" s="26">
-        <f>((2*9.81*1000*D8)/1.225)^0.5</f>
-        <v>11.932524580202749</v>
-      </c>
-      <c r="F8" s="26">
+      <c r="E8" s="25">
+        <f t="shared" si="3"/>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F8" s="25">
         <v>4060</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="25">
         <v>1.45</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="26" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="7">
@@ -1153,183 +1149,185 @@
         <f t="shared" si="0"/>
         <v>5.3339999999999999E-2</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="8">
         <f t="shared" si="1"/>
-        <v>29.228596564714788</v>
+        <v>29.417718019344075</v>
       </c>
       <c r="N8" s="8">
         <v>0.47</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <v>3760</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>2</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="25">
         <v>1.35</v>
       </c>
-      <c r="D9" s="26">
-        <f>(B9-C9)*0.0254</f>
+      <c r="D9" s="25">
+        <f t="shared" si="2"/>
         <v>1.6509999999999997E-2</v>
       </c>
-      <c r="E9" s="26">
-        <f>((2*9.81*1000*D9)/1.225)^0.5</f>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F9" s="26">
+      <c r="E9" s="25">
+        <f t="shared" si="3"/>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F9" s="25">
         <v>4130</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="25">
         <v>1.48</v>
       </c>
-      <c r="H9" s="27"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="25">
         <v>1.5</v>
       </c>
-      <c r="D10" s="26">
-        <f>(B10-C10)*0.0254</f>
+      <c r="D10" s="25">
+        <f t="shared" si="2"/>
         <v>2.4130000000000002E-2</v>
       </c>
-      <c r="E10" s="26">
-        <f>((2*9.81*1000*D10)/1.225)^0.5</f>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F10" s="26">
+      <c r="E10" s="25">
+        <f t="shared" si="3"/>
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F10" s="25">
         <v>3930</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="25">
         <v>1.27</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="25">
+      <c r="B11" s="24">
         <v>3</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>1.6</v>
       </c>
-      <c r="D11" s="26">
-        <f>(B11-C11)*0.0254</f>
+      <c r="D11" s="25">
+        <f t="shared" si="2"/>
         <v>3.5559999999999994E-2</v>
       </c>
-      <c r="E11" s="26">
-        <f>((2*9.81*1000*D11)/1.225)^0.5</f>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F11" s="26">
+      <c r="E11" s="25">
+        <f t="shared" si="3"/>
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F11" s="25">
         <v>4000</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="25">
         <v>1.17</v>
       </c>
-      <c r="H11" s="27"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="28">
+      <c r="B12" s="27">
         <v>1.65</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="28">
         <v>1.3</v>
       </c>
-      <c r="D12" s="29">
-        <f>(B12-C12)*0.0254</f>
+      <c r="D12" s="28">
+        <f t="shared" si="2"/>
         <v>8.8899999999999969E-3</v>
       </c>
-      <c r="E12" s="29">
-        <f>((2*9.81*1000*D12)/1.225)^0.5</f>
-        <v>11.932524580202749</v>
-      </c>
-      <c r="F12" s="29">
+      <c r="E12" s="28">
+        <f t="shared" si="3"/>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F12" s="28">
         <v>6000</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="28">
         <v>1.96</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="28">
+      <c r="B13" s="27">
         <v>2</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <v>1.35</v>
       </c>
-      <c r="D13" s="29">
-        <f>(B13-C13)*0.0254</f>
+      <c r="D13" s="28">
+        <f t="shared" si="2"/>
         <v>1.6509999999999997E-2</v>
       </c>
-      <c r="E13" s="29">
-        <f>((2*9.81*1000*D13)/1.225)^0.5</f>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F13" s="29">
+      <c r="E13" s="28">
+        <f t="shared" si="3"/>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F13" s="28">
         <v>5960</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="28">
         <v>2.2799999999999998</v>
       </c>
-      <c r="H13" s="30"/>
+      <c r="H13" s="29"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="28">
+      <c r="B14" s="27">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>1.5</v>
       </c>
-      <c r="D14" s="29">
-        <f>(B14-C14)*0.0254</f>
+      <c r="D14" s="28">
+        <f t="shared" si="2"/>
         <v>2.4130000000000002E-2</v>
       </c>
-      <c r="E14" s="29">
-        <f>((2*9.81*1000*D14)/1.225)^0.5</f>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F14" s="29">
+      <c r="E14" s="28">
+        <f t="shared" si="3"/>
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F14" s="28">
         <v>5950</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="28">
         <v>2.31</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="31">
+      <c r="B15" s="30">
         <v>3</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <v>1.6</v>
       </c>
-      <c r="D15" s="32">
-        <f>(B15-C15)*0.0254</f>
+      <c r="D15" s="31">
+        <f t="shared" si="2"/>
         <v>3.5559999999999994E-2</v>
       </c>
-      <c r="E15" s="32">
-        <f>((2*9.81*1000*D15)/1.225)^0.5</f>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F15" s="32">
+      <c r="E15" s="31">
+        <f t="shared" si="3"/>
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F15" s="31">
         <v>5870</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="31">
         <v>2.11</v>
       </c>
-      <c r="H15" s="33"/>
+      <c r="H15" s="32"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1339,308 +1337,316 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <f xml:space="preserve"> 1.2093</f>
+        <v>1.2093</v>
+      </c>
+    </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="38" t="s">
+      <c r="B18" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="40"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="41">
+      <c r="B19" s="40">
         <v>1.65</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="41">
         <v>1.3</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="41">
         <f>(B19-C19)*0.0254</f>
         <v>8.8899999999999969E-3</v>
       </c>
-      <c r="E19" s="42">
-        <f>((2*9.81*1000*D19)/1.225)^0.5</f>
-        <v>11.932524580202749</v>
-      </c>
-      <c r="F19" s="42">
+      <c r="E19" s="41">
+        <f>((2*9.81*1000*D19)/1.2093)^0.5</f>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F19" s="41">
         <v>3200</v>
       </c>
-      <c r="G19" s="42">
+      <c r="G19" s="41">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="42" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="41">
+      <c r="B20" s="40">
         <v>2</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="41">
         <v>1.35</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="41">
         <f>(B20-C20)*0.0254</f>
         <v>1.6509999999999997E-2</v>
       </c>
-      <c r="E20" s="42">
-        <f t="shared" ref="E20:E30" si="2">((2*9.81*1000*D20)/1.225)^0.5</f>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="44"/>
+      <c r="E20" s="41">
+        <f t="shared" ref="E20:E30" si="4">((2*9.81*1000*D20)/1.2093)^0.5</f>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="43"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="41">
+      <c r="B21" s="40">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="41">
         <v>1.5</v>
       </c>
-      <c r="D21" s="42">
-        <f t="shared" ref="D21:D30" si="3">(B21-C21)*0.0254</f>
+      <c r="D21" s="41">
+        <f t="shared" ref="D21:D30" si="5">(B21-C21)*0.0254</f>
         <v>2.4130000000000002E-2</v>
       </c>
-      <c r="E21" s="42">
-        <f t="shared" si="2"/>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F21" s="42">
+      <c r="E21" s="41">
+        <f t="shared" si="4"/>
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F21" s="41">
         <v>3291</v>
       </c>
-      <c r="G21" s="42">
+      <c r="G21" s="41">
         <v>10.130000000000001</v>
       </c>
-      <c r="H21" s="44"/>
+      <c r="H21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="41">
+      <c r="B22" s="40">
         <v>3</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="41">
         <v>1.6</v>
       </c>
-      <c r="D22" s="42">
-        <f t="shared" si="3"/>
+      <c r="D22" s="41">
+        <f t="shared" si="5"/>
         <v>3.5559999999999994E-2</v>
       </c>
-      <c r="E22" s="42">
-        <f t="shared" si="2"/>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F22" s="42">
+      <c r="E22" s="41">
+        <f t="shared" si="4"/>
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F22" s="41">
         <v>3100</v>
       </c>
-      <c r="G22" s="42">
+      <c r="G22" s="41">
         <v>10.25</v>
       </c>
-      <c r="H22" s="44"/>
+      <c r="H22" s="43"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="45">
+      <c r="B23" s="44">
         <v>1.65</v>
       </c>
-      <c r="C23" s="46">
+      <c r="C23" s="45">
         <v>1.3</v>
       </c>
-      <c r="D23" s="46">
-        <f t="shared" si="3"/>
+      <c r="D23" s="45">
+        <f t="shared" si="5"/>
         <v>8.8899999999999969E-3</v>
       </c>
-      <c r="E23" s="46">
-        <f t="shared" si="2"/>
-        <v>11.932524580202749</v>
-      </c>
-      <c r="F23" s="46">
+      <c r="E23" s="45">
+        <f t="shared" si="4"/>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F23" s="45">
         <v>4940</v>
       </c>
-      <c r="G23" s="46">
+      <c r="G23" s="45">
         <v>3.17</v>
       </c>
-      <c r="H23" s="47" t="s">
+      <c r="H23" s="46" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="45">
+      <c r="B24" s="44">
         <v>2</v>
       </c>
-      <c r="C24" s="46">
+      <c r="C24" s="45">
         <v>1.35</v>
       </c>
-      <c r="D24" s="46">
-        <f t="shared" si="3"/>
+      <c r="D24" s="45">
+        <f t="shared" si="5"/>
         <v>1.6509999999999997E-2</v>
       </c>
-      <c r="E24" s="46">
-        <f t="shared" si="2"/>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="48"/>
+      <c r="E24" s="45">
+        <f t="shared" si="4"/>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="47"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="45">
+      <c r="B25" s="44">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C25" s="46">
+      <c r="C25" s="45">
         <v>1.5</v>
       </c>
-      <c r="D25" s="46">
-        <f t="shared" si="3"/>
+      <c r="D25" s="45">
+        <f t="shared" si="5"/>
         <v>2.4130000000000002E-2</v>
       </c>
-      <c r="E25" s="46">
-        <f t="shared" si="2"/>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F25" s="46">
+      <c r="E25" s="45">
+        <f t="shared" si="4"/>
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F25" s="45">
         <v>4700</v>
       </c>
-      <c r="G25" s="46">
+      <c r="G25" s="45">
         <v>21.92</v>
       </c>
-      <c r="H25" s="48"/>
+      <c r="H25" s="47"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="45">
+      <c r="B26" s="44">
         <v>3</v>
       </c>
-      <c r="C26" s="46">
+      <c r="C26" s="45">
         <v>1.6</v>
       </c>
-      <c r="D26" s="46">
-        <f t="shared" si="3"/>
+      <c r="D26" s="45">
+        <f t="shared" si="5"/>
         <v>3.5559999999999994E-2</v>
       </c>
-      <c r="E26" s="46">
-        <f t="shared" si="2"/>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F26" s="46">
+      <c r="E26" s="45">
+        <f t="shared" si="4"/>
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F26" s="45">
         <v>4860</v>
       </c>
-      <c r="G26" s="46">
+      <c r="G26" s="45">
         <v>13.11</v>
       </c>
-      <c r="H26" s="48"/>
+      <c r="H26" s="47"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="49">
+      <c r="B27" s="48">
         <v>1.65</v>
       </c>
-      <c r="C27" s="50">
+      <c r="C27" s="49">
         <v>1.3</v>
       </c>
-      <c r="D27" s="50">
-        <f t="shared" si="3"/>
+      <c r="D27" s="49">
+        <f t="shared" si="5"/>
         <v>8.8899999999999969E-3</v>
       </c>
-      <c r="E27" s="50">
-        <f t="shared" si="2"/>
-        <v>11.932524580202749</v>
-      </c>
-      <c r="F27" s="50">
+      <c r="E27" s="49">
+        <f t="shared" si="4"/>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F27" s="49">
         <v>5800</v>
       </c>
-      <c r="G27" s="50">
+      <c r="G27" s="49">
         <v>1.65</v>
       </c>
-      <c r="H27" s="51" t="s">
+      <c r="H27" s="50" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="49">
+      <c r="B28" s="48">
         <v>2</v>
       </c>
-      <c r="C28" s="50">
+      <c r="C28" s="49">
         <v>1.35</v>
       </c>
-      <c r="D28" s="50">
-        <f t="shared" si="3"/>
+      <c r="D28" s="49">
+        <f t="shared" si="5"/>
         <v>1.6509999999999997E-2</v>
       </c>
-      <c r="E28" s="50">
-        <f t="shared" si="2"/>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="52"/>
+      <c r="E28" s="49">
+        <f t="shared" si="4"/>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="51"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="49">
+      <c r="B29" s="48">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C29" s="50">
+      <c r="C29" s="49">
         <v>1.5</v>
       </c>
-      <c r="D29" s="50">
-        <f t="shared" si="3"/>
+      <c r="D29" s="49">
+        <f t="shared" si="5"/>
         <v>2.4130000000000002E-2</v>
       </c>
-      <c r="E29" s="50">
-        <f t="shared" si="2"/>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F29" s="50">
+      <c r="E29" s="49">
+        <f t="shared" si="4"/>
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F29" s="49">
         <v>5844</v>
       </c>
-      <c r="G29" s="50">
+      <c r="G29" s="49">
         <v>13.91</v>
       </c>
-      <c r="H29" s="52"/>
+      <c r="H29" s="51"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="53">
+      <c r="B30" s="52">
         <v>3</v>
       </c>
-      <c r="C30" s="54">
+      <c r="C30" s="53">
         <v>1.6</v>
       </c>
-      <c r="D30" s="54">
-        <f t="shared" si="3"/>
+      <c r="D30" s="53">
+        <f t="shared" si="5"/>
         <v>3.5559999999999994E-2</v>
       </c>
-      <c r="E30" s="54">
-        <f t="shared" si="2"/>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F30" s="54">
+      <c r="E30" s="53">
+        <f t="shared" si="4"/>
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F30" s="53">
         <v>5916</v>
       </c>
-      <c r="G30" s="54">
+      <c r="G30" s="53">
         <v>8.9700000000000006</v>
       </c>
-      <c r="H30" s="55"/>
+      <c r="H30" s="54"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
@@ -1651,318 +1657,318 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="58"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="57"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="60" t="s">
+      <c r="B33" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="60" t="s">
+      <c r="E33" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="60" t="s">
+      <c r="F33" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="G33" s="60" t="s">
+      <c r="G33" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="61"/>
+      <c r="H33" s="60"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="41">
+      <c r="B34" s="40">
         <v>1.65</v>
       </c>
-      <c r="C34" s="42">
+      <c r="C34" s="41">
         <v>1.3</v>
       </c>
-      <c r="D34" s="42">
-        <f t="shared" ref="D34:D41" si="4">(B34-C34)*0.0254</f>
+      <c r="D34" s="41">
+        <f t="shared" ref="D34:D41" si="6">(B34-C34)*0.0254</f>
         <v>8.8899999999999969E-3</v>
       </c>
-      <c r="E34" s="42">
-        <f t="shared" ref="E34:E41" si="5">((2*9.81*1000*D34)/1.225)^0.5</f>
-        <v>11.932524580202749</v>
-      </c>
-      <c r="F34" s="42">
+      <c r="E34" s="41">
+        <f>((2*9.81*1000*D34)/1.2093)^0.5</f>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F34" s="41">
         <v>3720</v>
       </c>
-      <c r="G34" s="42">
+      <c r="G34" s="41">
         <v>3.72</v>
       </c>
-      <c r="H34" s="43" t="s">
+      <c r="H34" s="42" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="41">
+      <c r="B35" s="40">
         <v>2</v>
       </c>
-      <c r="C35" s="42">
+      <c r="C35" s="41">
         <v>1.35</v>
       </c>
-      <c r="D35" s="42">
-        <f t="shared" si="4"/>
-        <v>1.6509999999999997E-2</v>
-      </c>
-      <c r="E35" s="42">
-        <f t="shared" si="5"/>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F35" s="42">
-        <v>3660</v>
-      </c>
-      <c r="G35" s="42">
-        <v>6</v>
-      </c>
-      <c r="H35" s="44"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="41">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="C36" s="42">
-        <v>1.5</v>
-      </c>
-      <c r="D36" s="42">
-        <f t="shared" si="4"/>
-        <v>2.4130000000000002E-2</v>
-      </c>
-      <c r="E36" s="42">
-        <f t="shared" si="5"/>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F36" s="42">
-        <v>3675</v>
-      </c>
-      <c r="G36" s="42">
-        <v>8.42</v>
-      </c>
-      <c r="H36" s="44"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="41">
-        <v>3</v>
-      </c>
-      <c r="C37" s="42">
-        <v>1.6</v>
-      </c>
-      <c r="D37" s="42">
-        <f t="shared" si="4"/>
-        <v>3.5559999999999994E-2</v>
-      </c>
-      <c r="E37" s="42">
-        <f t="shared" si="5"/>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F37" s="42">
-        <v>3000</v>
-      </c>
-      <c r="G37" s="42">
-        <v>10.6</v>
-      </c>
-      <c r="H37" s="44"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="62">
-        <v>1.65</v>
-      </c>
-      <c r="C38" s="63">
-        <v>1.3</v>
-      </c>
-      <c r="D38" s="46">
-        <f t="shared" si="4"/>
-        <v>8.8899999999999969E-3</v>
-      </c>
-      <c r="E38" s="46">
-        <f t="shared" si="5"/>
-        <v>11.932524580202749</v>
-      </c>
-      <c r="F38" s="63">
-        <v>4560</v>
-      </c>
-      <c r="G38" s="63">
-        <v>3.14</v>
-      </c>
-      <c r="H38" s="47" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="62">
-        <v>2</v>
-      </c>
-      <c r="C39" s="63">
-        <v>1.35</v>
-      </c>
-      <c r="D39" s="46">
-        <f t="shared" si="4"/>
-        <v>1.6509999999999997E-2</v>
-      </c>
-      <c r="E39" s="46">
-        <f t="shared" si="5"/>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F39" s="63">
-        <v>4470</v>
-      </c>
-      <c r="G39" s="63">
-        <v>4.97</v>
-      </c>
-      <c r="H39" s="48"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="62">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="C40" s="63">
-        <v>1.5</v>
-      </c>
-      <c r="D40" s="46">
-        <f t="shared" si="4"/>
-        <v>2.4130000000000002E-2</v>
-      </c>
-      <c r="E40" s="46">
-        <f t="shared" si="5"/>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F40" s="63">
-        <v>4050</v>
-      </c>
-      <c r="G40" s="63">
-        <v>7.25</v>
-      </c>
-      <c r="H40" s="48"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="62">
-        <v>3</v>
-      </c>
-      <c r="C41" s="63">
-        <v>1.6</v>
-      </c>
-      <c r="D41" s="46">
-        <f t="shared" si="4"/>
-        <v>3.5559999999999994E-2</v>
-      </c>
-      <c r="E41" s="46">
-        <f t="shared" si="5"/>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F41" s="63">
-        <v>3160</v>
-      </c>
-      <c r="G41" s="63">
-        <v>15.5</v>
-      </c>
-      <c r="H41" s="48"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="64">
-        <v>1.65</v>
-      </c>
-      <c r="C42" s="65">
-        <v>1.3</v>
-      </c>
-      <c r="D42" s="65">
-        <f t="shared" ref="D42:D45" si="6">(B42-C42)*0.0254</f>
-        <v>8.8899999999999969E-3</v>
-      </c>
-      <c r="E42" s="65">
-        <f t="shared" ref="E42:E45" si="7">((2*9.81*1000*D42)/1.225)^0.5</f>
-        <v>11.932524580202749</v>
-      </c>
-      <c r="F42" s="65">
-        <v>5560</v>
-      </c>
-      <c r="G42" s="65">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="H42" s="51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="64">
-        <v>2</v>
-      </c>
-      <c r="C43" s="65">
-        <v>1.35</v>
-      </c>
-      <c r="D43" s="65">
+      <c r="D35" s="41">
         <f t="shared" si="6"/>
         <v>1.6509999999999997E-2</v>
       </c>
-      <c r="E43" s="65">
-        <f t="shared" si="7"/>
-        <v>16.261289955609552</v>
-      </c>
-      <c r="F43" s="65">
-        <v>5630</v>
-      </c>
-      <c r="G43" s="65">
-        <v>5.26</v>
-      </c>
-      <c r="H43" s="52"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="64">
+      <c r="E35" s="41">
+        <f t="shared" ref="E35:E45" si="7">((2*9.81*1000*D35)/1.2093)^0.5</f>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F35" s="41">
+        <v>3660</v>
+      </c>
+      <c r="G35" s="41">
+        <v>6</v>
+      </c>
+      <c r="H35" s="43"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="40">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C44" s="65">
+      <c r="C36" s="41">
         <v>1.5</v>
       </c>
-      <c r="D44" s="65">
+      <c r="D36" s="41">
         <f t="shared" si="6"/>
         <v>2.4130000000000002E-2</v>
       </c>
-      <c r="E44" s="65">
+      <c r="E36" s="41">
         <f t="shared" si="7"/>
-        <v>19.658940947662298</v>
-      </c>
-      <c r="F44" s="65">
-        <v>5500</v>
-      </c>
-      <c r="G44" s="65">
-        <v>7.67</v>
-      </c>
-      <c r="H44" s="52"/>
-    </row>
-    <row r="45" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="66">
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F36" s="41">
+        <v>3675</v>
+      </c>
+      <c r="G36" s="41">
+        <v>8.42</v>
+      </c>
+      <c r="H36" s="43"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="40">
         <v>3</v>
       </c>
-      <c r="C45" s="67">
+      <c r="C37" s="41">
         <v>1.6</v>
       </c>
-      <c r="D45" s="67">
+      <c r="D37" s="41">
         <f t="shared" si="6"/>
         <v>3.5559999999999994E-2</v>
       </c>
-      <c r="E45" s="67">
+      <c r="E37" s="41">
         <f t="shared" si="7"/>
-        <v>23.865049160405501</v>
-      </c>
-      <c r="F45" s="67">
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F37" s="41">
+        <v>3000</v>
+      </c>
+      <c r="G37" s="41">
+        <v>10.6</v>
+      </c>
+      <c r="H37" s="43"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="61">
+        <v>1.65</v>
+      </c>
+      <c r="C38" s="62">
+        <v>1.3</v>
+      </c>
+      <c r="D38" s="45">
+        <f t="shared" si="6"/>
+        <v>8.8899999999999969E-3</v>
+      </c>
+      <c r="E38" s="45">
+        <f t="shared" si="7"/>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F38" s="62">
+        <v>4560</v>
+      </c>
+      <c r="G38" s="62">
+        <v>3.14</v>
+      </c>
+      <c r="H38" s="46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="61">
+        <v>2</v>
+      </c>
+      <c r="C39" s="62">
+        <v>1.35</v>
+      </c>
+      <c r="D39" s="45">
+        <f t="shared" si="6"/>
+        <v>1.6509999999999997E-2</v>
+      </c>
+      <c r="E39" s="45">
+        <f t="shared" si="7"/>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F39" s="62">
+        <v>4470</v>
+      </c>
+      <c r="G39" s="62">
+        <v>4.97</v>
+      </c>
+      <c r="H39" s="47"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="61">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C40" s="62">
+        <v>1.5</v>
+      </c>
+      <c r="D40" s="45">
+        <f t="shared" si="6"/>
+        <v>2.4130000000000002E-2</v>
+      </c>
+      <c r="E40" s="45">
+        <f t="shared" si="7"/>
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F40" s="62">
+        <v>4050</v>
+      </c>
+      <c r="G40" s="62">
+        <v>7.25</v>
+      </c>
+      <c r="H40" s="47"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="61">
+        <v>3</v>
+      </c>
+      <c r="C41" s="62">
+        <v>1.6</v>
+      </c>
+      <c r="D41" s="45">
+        <f t="shared" si="6"/>
+        <v>3.5559999999999994E-2</v>
+      </c>
+      <c r="E41" s="45">
+        <f t="shared" si="7"/>
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F41" s="62">
+        <v>3160</v>
+      </c>
+      <c r="G41" s="62">
+        <v>15.5</v>
+      </c>
+      <c r="H41" s="47"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="63">
+        <v>1.65</v>
+      </c>
+      <c r="C42" s="64">
+        <v>1.3</v>
+      </c>
+      <c r="D42" s="64">
+        <f t="shared" ref="D42:D45" si="8">(B42-C42)*0.0254</f>
+        <v>8.8899999999999969E-3</v>
+      </c>
+      <c r="E42" s="64">
+        <f t="shared" si="7"/>
+        <v>12.009733090745195</v>
+      </c>
+      <c r="F42" s="64">
+        <v>5560</v>
+      </c>
+      <c r="G42" s="64">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="H42" s="50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="63">
+        <v>2</v>
+      </c>
+      <c r="C43" s="64">
+        <v>1.35</v>
+      </c>
+      <c r="D43" s="64">
+        <f t="shared" si="8"/>
+        <v>1.6509999999999997E-2</v>
+      </c>
+      <c r="E43" s="64">
+        <f t="shared" si="7"/>
+        <v>16.366507419737342</v>
+      </c>
+      <c r="F43" s="64">
+        <v>5630</v>
+      </c>
+      <c r="G43" s="64">
+        <v>5.26</v>
+      </c>
+      <c r="H43" s="51"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="63">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C44" s="64">
+        <v>1.5</v>
+      </c>
+      <c r="D44" s="64">
+        <f t="shared" si="8"/>
+        <v>2.4130000000000002E-2</v>
+      </c>
+      <c r="E44" s="64">
+        <f t="shared" si="7"/>
+        <v>19.786142659186879</v>
+      </c>
+      <c r="F44" s="64">
+        <v>5500</v>
+      </c>
+      <c r="G44" s="64">
+        <v>7.67</v>
+      </c>
+      <c r="H44" s="51"/>
+    </row>
+    <row r="45" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="65">
+        <v>3</v>
+      </c>
+      <c r="C45" s="66">
+        <v>1.6</v>
+      </c>
+      <c r="D45" s="66">
+        <f t="shared" si="8"/>
+        <v>3.5559999999999994E-2</v>
+      </c>
+      <c r="E45" s="66">
+        <f t="shared" si="7"/>
+        <v>24.019466181490394</v>
+      </c>
+      <c r="F45" s="66">
         <v>5200</v>
       </c>
-      <c r="G45" s="67">
+      <c r="G45" s="66">
         <v>10.43</v>
       </c>
-      <c r="H45" s="55"/>
+      <c r="H45" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
plots and codes updated'
</commit_message>
<xml_diff>
--- a/Analysis Codes/Experimental Data.xlsx
+++ b/Analysis Codes/Experimental Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\ME201617\ME Spring 2017\Final project\Analysis Codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ME201617\ME Spring 2017\Final project\Analysis Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -847,8 +847,8 @@
   </sheetPr>
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>